<commit_message>
update srf data map entry, update whoiswho
</commit_message>
<xml_diff>
--- a/whoiswho/whoiswho.xlsx
+++ b/whoiswho/whoiswho.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kira\OneDrive\SHK WiJo\wijou\whoiswho\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22110" windowHeight="9555"/>
   </bookViews>
   <sheets>
     <sheet name="whoiswho" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="251">
   <si>
     <t>bild</t>
   </si>
@@ -79,18 +84,9 @@
     <t>Sylke Gruhnwald</t>
   </si>
   <si>
-    <t>Leiterin SRF Data Team</t>
-  </si>
-  <si>
     <t>Zürich</t>
   </si>
   <si>
-    <t>SRF Data</t>
-  </si>
-  <si>
-    <t>http://www.srf.ch/news/srf-data</t>
-  </si>
-  <si>
     <t>@SylkeGruhnwald</t>
   </si>
   <si>
@@ -662,13 +658,130 @@
   </si>
   <si>
     <t>Datenjournalist, ZEIT Online</t>
+  </si>
+  <si>
+    <t>julianschmidli.com</t>
+  </si>
+  <si>
+    <t>http://www.mirkolorenz.com/</t>
+  </si>
+  <si>
+    <t>mirkolorenz.com</t>
+  </si>
+  <si>
+    <t>David Bauer</t>
+  </si>
+  <si>
+    <t>Bernd Oswald</t>
+  </si>
+  <si>
+    <t>Leiter NZZ Storytelling</t>
+  </si>
+  <si>
+    <t>Datenjournalismus-Trainer</t>
+  </si>
+  <si>
+    <t>@davidbauer</t>
+  </si>
+  <si>
+    <t>@berndoswald</t>
+  </si>
+  <si>
+    <t>https://twitter.com/berndoswald</t>
+  </si>
+  <si>
+    <t>http://www.journalisten-training.de/</t>
+  </si>
+  <si>
+    <t>Journalisten-Training</t>
+  </si>
+  <si>
+    <t>http://t.co/kgWVRXI5RD</t>
+  </si>
+  <si>
+    <t>davidbauer.ch</t>
+  </si>
+  <si>
+    <t>https://twitter.com/davidbauer</t>
+  </si>
+  <si>
+    <t>Vanessa Wormer</t>
+  </si>
+  <si>
+    <t>Investigative Datenjournalistin, Süddeutsche Zeitung</t>
+  </si>
+  <si>
+    <t>vanessawormer.de</t>
+  </si>
+  <si>
+    <t>http://www.vanessawormer.de/</t>
+  </si>
+  <si>
+    <t>@Remrow</t>
+  </si>
+  <si>
+    <t>https://twitter.com/Remrow</t>
+  </si>
+  <si>
+    <t>Achim Tack</t>
+  </si>
+  <si>
+    <t>Moritz Klack</t>
+  </si>
+  <si>
+    <t>Marcel Pauly</t>
+  </si>
+  <si>
+    <t>http://www.achim-tack.org/</t>
+  </si>
+  <si>
+    <t>achimtack.org</t>
+  </si>
+  <si>
+    <t>https://twitter.com/A_Tack</t>
+  </si>
+  <si>
+    <t>@A_Tack</t>
+  </si>
+  <si>
+    <t>webkid.io</t>
+  </si>
+  <si>
+    <t>http://webkid.io/</t>
+  </si>
+  <si>
+    <t>@moklick</t>
+  </si>
+  <si>
+    <t>Interaktiv-Team, Berliner Morgenpost | Gründer Webkid.io</t>
+  </si>
+  <si>
+    <t>https://twitter.com/moklick</t>
+  </si>
+  <si>
+    <t>https://twitter.com/marcelpauly</t>
+  </si>
+  <si>
+    <t>@marcelpauly</t>
+  </si>
+  <si>
+    <t>http://www.marcelpauly.de/</t>
+  </si>
+  <si>
+    <t>marcelpauly.de</t>
+  </si>
+  <si>
+    <t>Datenjournalist, Investivatig-Team, Welt-Gruppe</t>
+  </si>
+  <si>
+    <t>Berlin/Hamburg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -804,6 +917,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1102,7 +1223,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1145,12 +1266,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1181,6 +1304,7 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1228,14 +1352,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1273,9 +1400,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1310,7 +1437,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1345,7 +1472,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1519,21 +1646,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="32.21875" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="1"/>
-    <col min="9" max="9" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1552,7 +1679,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1565,7 +1692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>10</v>
       </c>
@@ -1581,7 +1708,7 @@
       <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1594,736 +1721,880 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
         <v>196</v>
       </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
         <v>197</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
         <v>198</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="D10" t="s">
         <v>70</v>
       </c>
-      <c r="J9" t="s">
+      <c r="E10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="F10" t="s">
         <v>72</v>
       </c>
-      <c r="C10" t="s">
-        <v>201</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="G10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>74</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="J10" t="s">
         <v>76</v>
       </c>
-      <c r="H10" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>77</v>
-      </c>
-      <c r="I10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>82</v>
       </c>
-      <c r="G11" t="s">
+      <c r="J11" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>84</v>
       </c>
-      <c r="I11" t="s">
+      <c r="C12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" t="s">
         <v>85</v>
       </c>
-      <c r="J11" t="s">
+      <c r="E12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="F12" t="s">
         <v>87</v>
       </c>
-      <c r="C12" t="s">
-        <v>202</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="G12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
         <v>89</v>
       </c>
-      <c r="F12" t="s">
+      <c r="I12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="J12" t="s">
         <v>91</v>
       </c>
-      <c r="H12" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>92</v>
       </c>
-      <c r="I12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
       <c r="C13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="I13" t="s">
         <v>97</v>
       </c>
-      <c r="G13" t="s">
+      <c r="J13" t="s">
         <v>98</v>
       </c>
-      <c r="H13" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>99</v>
       </c>
-      <c r="I13" t="s">
+      <c r="C14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
         <v>100</v>
       </c>
-      <c r="J13" t="s">
+      <c r="F14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="G14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C14" t="s">
-        <v>208</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>103</v>
       </c>
-      <c r="F14" t="s">
+      <c r="I14" t="s">
         <v>104</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="J14" t="s">
         <v>105</v>
       </c>
-      <c r="H14" t="s">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>106</v>
       </c>
-      <c r="I14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>109</v>
-      </c>
       <c r="C15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" t="s">
         <v>110</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="J15" t="s">
         <v>112</v>
       </c>
-      <c r="H15" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>113</v>
       </c>
-      <c r="I15" t="s">
+      <c r="C16" t="s">
         <v>114</v>
-      </c>
-      <c r="J15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" t="s">
-        <v>117</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F16" t="s">
+      <c r="I16" t="s">
         <v>119</v>
       </c>
-      <c r="G16" t="s">
+      <c r="J16" t="s">
         <v>120</v>
       </c>
-      <c r="H16" s="1" t="s">
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>121</v>
       </c>
-      <c r="I16" t="s">
+      <c r="C17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J16" t="s">
+      <c r="H17" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="I17" t="s">
         <v>124</v>
       </c>
-      <c r="C17" t="s">
-        <v>205</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="J17" t="s">
         <v>125</v>
       </c>
-      <c r="H17" t="s">
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>126</v>
       </c>
-      <c r="I17" t="s">
+      <c r="C18" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
         <v>127</v>
       </c>
-      <c r="J17" t="s">
+      <c r="F18" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="G18" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C18" t="s">
-        <v>205</v>
-      </c>
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="H18" t="s">
         <v>130</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="J18" t="s">
         <v>132</v>
       </c>
-      <c r="H18" t="s">
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>133</v>
       </c>
-      <c r="I18" t="s">
+      <c r="C19" t="s">
+        <v>203</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
         <v>134</v>
       </c>
-      <c r="J18" t="s">
+      <c r="F19" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="G19" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C19" t="s">
-        <v>206</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="H19" t="s">
         <v>137</v>
       </c>
-      <c r="F19" t="s">
+      <c r="I19" t="s">
         <v>138</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="J19" t="s">
         <v>139</v>
       </c>
-      <c r="H19" t="s">
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>140</v>
       </c>
-      <c r="I19" t="s">
+      <c r="C20" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" t="s">
         <v>141</v>
       </c>
-      <c r="J19" t="s">
+      <c r="E20" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="F20" t="s">
         <v>143</v>
       </c>
-      <c r="C20" t="s">
-        <v>207</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="G20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
         <v>145</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>146</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="J20" t="s">
         <v>147</v>
       </c>
-      <c r="H20" t="s">
-        <v>148</v>
-      </c>
-      <c r="I20" t="s">
-        <v>149</v>
-      </c>
-      <c r="J20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H21" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I21" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J21" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>212</v>
+      </c>
+      <c r="F22" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H22" t="s">
         <v>151</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F24" t="s">
+        <v>213</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" t="s">
+        <v>208</v>
+      </c>
+      <c r="D25" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" t="s">
         <v>209</v>
       </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" t="s">
-        <v>152</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>155</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D26" t="s">
+        <v>161</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" t="s">
+        <v>161</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" t="s">
+        <v>209</v>
+      </c>
+      <c r="D29" t="s">
+        <v>161</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" t="s">
+        <v>209</v>
+      </c>
+      <c r="D30" t="s">
+        <v>161</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" t="s">
         <v>210</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="H23" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>158</v>
-      </c>
-      <c r="C24" t="s">
-        <v>159</v>
-      </c>
-      <c r="D24" t="s">
-        <v>160</v>
-      </c>
-      <c r="G24" t="s">
-        <v>161</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>163</v>
-      </c>
-      <c r="C25" t="s">
-        <v>211</v>
-      </c>
-      <c r="D25" t="s">
-        <v>164</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>167</v>
-      </c>
-      <c r="C26" t="s">
-        <v>212</v>
-      </c>
-      <c r="D26" t="s">
-        <v>164</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>170</v>
-      </c>
-      <c r="C27" t="s">
-        <v>212</v>
-      </c>
-      <c r="D27" t="s">
-        <v>164</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H27" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" t="s">
-        <v>212</v>
-      </c>
-      <c r="D28" t="s">
-        <v>164</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H28" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>176</v>
-      </c>
-      <c r="C29" t="s">
-        <v>212</v>
-      </c>
-      <c r="D29" t="s">
-        <v>164</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>179</v>
-      </c>
-      <c r="C30" t="s">
-        <v>212</v>
-      </c>
-      <c r="D30" t="s">
-        <v>164</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>182</v>
-      </c>
-      <c r="C31" t="s">
-        <v>213</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H31" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H32" t="s">
-        <v>187</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>215</v>
+      </c>
+      <c r="C33" t="s">
+        <v>217</v>
+      </c>
+      <c r="D33" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" t="s">
+        <v>225</v>
+      </c>
+      <c r="F33" t="s">
+        <v>224</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>216</v>
+      </c>
+      <c r="C34" t="s">
+        <v>218</v>
+      </c>
+      <c r="D34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" t="s">
+        <v>223</v>
+      </c>
+      <c r="F34" t="s">
+        <v>222</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>227</v>
+      </c>
+      <c r="C35" t="s">
+        <v>228</v>
+      </c>
+      <c r="D35" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" t="s">
+        <v>229</v>
+      </c>
+      <c r="F35" t="s">
+        <v>230</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>233</v>
+      </c>
+      <c r="C36" t="s">
+        <v>194</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>237</v>
+      </c>
+      <c r="F36" t="s">
+        <v>236</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" t="s">
+        <v>243</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>240</v>
+      </c>
+      <c r="F37" t="s">
+        <v>241</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" t="s">
+        <v>249</v>
+      </c>
+      <c r="D38" t="s">
+        <v>250</v>
+      </c>
+      <c r="E38" t="s">
+        <v>248</v>
+      </c>
+      <c r="F38" t="s">
+        <v>247</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H33" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>